<commit_message>
Sprint 1 burndown chart
</commit_message>
<xml_diff>
--- a/Sprint-Backlog-Burndown-Chart.xlsx
+++ b/Sprint-Backlog-Burndown-Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colinconway/Courses/Software_engineering/sandwichTruckProj./"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F9A93D-925F-C749-AB44-036DBE4ADD1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B04CE3-A1FF-8549-89DB-985C6A0233CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="880" windowWidth="25180" windowHeight="14860" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="45">
   <si>
     <t>User Story #1</t>
   </si>
@@ -140,9 +140,6 @@
     <t>User Story #4 (other)</t>
   </si>
   <si>
-    <t>Task: JavaDocs</t>
-  </si>
-  <si>
     <t>Task: Map</t>
   </si>
   <si>
@@ -155,22 +152,25 @@
     <t>Luke Suppa</t>
   </si>
   <si>
-    <t>Task:  create basch file</t>
-  </si>
-  <si>
     <t>Task; JavaDocs</t>
   </si>
   <si>
     <t>Task: GUI</t>
   </si>
   <si>
-    <t>Task: Testing and Map</t>
-  </si>
-  <si>
     <t>Jake Clause</t>
   </si>
   <si>
     <t xml:space="preserve">Task Random Houses </t>
+  </si>
+  <si>
+    <t>Task:  create batch  file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task: </t>
+  </si>
+  <si>
+    <t>Task Map</t>
   </si>
 </sst>
 </file>
@@ -348,6 +348,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -363,9 +366,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -715,19 +715,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>114</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>88</c:v>
+                  <c:v>86</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>78</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>53</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>38</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -1280,30 +1280,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:29" ht="50" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
       <c r="X1" s="4"/>
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
@@ -1315,19 +1315,19 @@
       <c r="B2" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
       <c r="N2" s="10"/>
       <c r="O2" s="10"/>
       <c r="P2" s="10"/>
@@ -5496,7 +5496,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J16" sqref="J16"/>
+      <selection pane="bottomLeft" activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5518,29 +5518,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:28" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="19"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="20"/>
+      <c r="S1" s="20"/>
+      <c r="T1" s="20"/>
+      <c r="U1" s="20"/>
+      <c r="V1" s="20"/>
       <c r="W1" s="4"/>
       <c r="X1" s="4"/>
       <c r="Y1" s="4"/>
@@ -5552,18 +5552,18 @@
       <c r="B2" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
       <c r="M2" s="12"/>
       <c r="N2" s="12"/>
       <c r="O2" s="12"/>
@@ -5665,11 +5665,11 @@
     </row>
     <row r="5" spans="2:28" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="14">
@@ -5679,15 +5679,17 @@
         <v>26</v>
       </c>
       <c r="H5" s="14">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="I5" s="14">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="J5" s="14">
-        <v>12</v>
-      </c>
-      <c r="K5" s="14"/>
+        <v>8</v>
+      </c>
+      <c r="K5" s="14">
+        <v>0</v>
+      </c>
       <c r="L5" s="9"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
@@ -5708,28 +5710,16 @@
     </row>
     <row r="6" spans="2:28" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="9" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C6" s="9"/>
-      <c r="D6" s="9" t="s">
-        <v>36</v>
-      </c>
+      <c r="D6" s="9"/>
       <c r="E6" s="9"/>
-      <c r="F6" s="14">
-        <v>2</v>
-      </c>
-      <c r="G6" s="14">
-        <v>2</v>
-      </c>
-      <c r="H6" s="14">
-        <v>2</v>
-      </c>
-      <c r="I6" s="14">
-        <v>1</v>
-      </c>
-      <c r="J6" s="14">
-        <v>1</v>
-      </c>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
       <c r="K6" s="14"/>
       <c r="L6" s="9"/>
       <c r="M6" s="4"/>
@@ -5751,11 +5741,11 @@
     </row>
     <row r="7" spans="2:28" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="13">
@@ -5771,9 +5761,11 @@
         <v>10</v>
       </c>
       <c r="J7" s="14">
-        <v>12</v>
-      </c>
-      <c r="K7" s="14"/>
+        <v>6</v>
+      </c>
+      <c r="K7" s="14">
+        <v>0</v>
+      </c>
       <c r="L7" s="9"/>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
@@ -5794,28 +5786,16 @@
     </row>
     <row r="8" spans="2:28" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="9" t="s">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="C8" s="9"/>
-      <c r="D8" s="9" t="s">
-        <v>38</v>
-      </c>
+      <c r="D8" s="9"/>
       <c r="E8" s="9"/>
-      <c r="F8" s="14">
-        <v>2</v>
-      </c>
-      <c r="G8" s="14">
-        <v>2</v>
-      </c>
-      <c r="H8" s="14">
-        <v>2</v>
-      </c>
-      <c r="I8" s="14">
-        <v>1</v>
-      </c>
-      <c r="J8" s="14">
-        <v>1</v>
-      </c>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
       <c r="K8" s="14"/>
       <c r="L8" s="9"/>
       <c r="M8" s="4"/>
@@ -5868,11 +5848,11 @@
     </row>
     <row r="10" spans="2:28" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="9">
@@ -5881,7 +5861,7 @@
       <c r="G10" s="9">
         <v>26</v>
       </c>
-      <c r="H10" s="21">
+      <c r="H10" s="15">
         <v>24</v>
       </c>
       <c r="I10" s="9">
@@ -5890,7 +5870,9 @@
       <c r="J10" s="9">
         <v>8</v>
       </c>
-      <c r="K10" s="9"/>
+      <c r="K10" s="9">
+        <v>0</v>
+      </c>
       <c r="L10" s="9"/>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
@@ -5911,14 +5893,12 @@
     </row>
     <row r="11" spans="2:28" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
-      <c r="F11" s="9">
-        <v>20</v>
-      </c>
+      <c r="F11" s="9"/>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
@@ -6037,11 +6017,11 @@
     </row>
     <row r="15" spans="2:28" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="9" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E15" s="9"/>
       <c r="F15" s="9">
@@ -6059,7 +6039,9 @@
       <c r="J15" s="9">
         <v>1</v>
       </c>
-      <c r="K15" s="9"/>
+      <c r="K15" s="9">
+        <v>0</v>
+      </c>
       <c r="L15" s="9"/>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
@@ -6080,11 +6062,11 @@
     </row>
     <row r="16" spans="2:28" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C16" s="9"/>
       <c r="D16" s="9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E16" s="9"/>
       <c r="F16" s="9">
@@ -6102,7 +6084,9 @@
       <c r="J16" s="9">
         <v>3</v>
       </c>
-      <c r="K16" s="9"/>
+      <c r="K16" s="9">
+        <v>0</v>
+      </c>
       <c r="L16" s="9"/>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
@@ -6219,14 +6203,28 @@
         <v>32</v>
       </c>
       <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
+      <c r="D20" s="9" t="s">
+        <v>37</v>
+      </c>
       <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
+      <c r="F20" s="9">
+        <v>2</v>
+      </c>
+      <c r="G20" s="9">
+        <v>2</v>
+      </c>
+      <c r="H20" s="9">
+        <v>2</v>
+      </c>
+      <c r="I20" s="9">
+        <v>1</v>
+      </c>
+      <c r="J20" s="9">
+        <v>1</v>
+      </c>
+      <c r="K20" s="9">
+        <v>0</v>
+      </c>
       <c r="L20" s="9"/>
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
@@ -6246,9 +6244,7 @@
       <c r="AB20" s="4"/>
     </row>
     <row r="21" spans="2:28" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="9" t="s">
-        <v>34</v>
-      </c>
+      <c r="B21" s="9"/>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
@@ -6502,23 +6498,23 @@
       <c r="E29" s="5"/>
       <c r="F29" s="5">
         <f>SUM(F4:F28)</f>
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="G29" s="5">
         <f>SUM(G5:G28)</f>
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H29" s="5">
         <f>SUM(H4:H28)</f>
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="I29" s="5">
         <f>SUM(I4:I28)</f>
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="J29" s="5">
         <f>SUM(J4:J28)</f>
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="K29" s="5">
         <f>SUM(K4:K28)</f>

</xml_diff>

<commit_message>
Sprint Burndown Chart Updated
</commit_message>
<xml_diff>
--- a/Sprint-Backlog-Burndown-Chart.xlsx
+++ b/Sprint-Backlog-Burndown-Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colinconway/Courses/Software_engineering/sandwichTruckProj./"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61ED5991-9BC4-0449-BDF5-AC8B217E1148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02212AA2-8FFE-FD49-A601-341ECD151B33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="880" windowWidth="25180" windowHeight="14860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="52">
   <si>
     <t>User Story #1</t>
   </si>
@@ -173,6 +173,27 @@
   </si>
   <si>
     <t>Task Map</t>
+  </si>
+  <si>
+    <t>Task Add Timestamps</t>
+  </si>
+  <si>
+    <t>Thursday 3/24</t>
+  </si>
+  <si>
+    <t>Tuesday 3/22</t>
+  </si>
+  <si>
+    <t>Thursday 3/17</t>
+  </si>
+  <si>
+    <t>Tuesday 3/15</t>
+  </si>
+  <si>
+    <t>Thursday 3/10</t>
+  </si>
+  <si>
+    <t>Tuesday 3/8</t>
   </si>
 </sst>
 </file>
@@ -498,10 +519,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1539,7 +1560,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F26" sqref="F26:M29"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1687,24 +1708,26 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="M4" s="6"/>
+        <v>46</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>46</v>
+      </c>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
@@ -1758,19 +1781,37 @@
     </row>
     <row r="6" spans="2:29" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="9" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
+      <c r="D6" s="9" t="s">
+        <v>35</v>
+      </c>
       <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
+      <c r="F6" s="9">
+        <v>2</v>
+      </c>
+      <c r="G6" s="9">
+        <v>2</v>
+      </c>
+      <c r="H6" s="9">
+        <v>0</v>
+      </c>
+      <c r="I6" s="9">
+        <v>0</v>
+      </c>
+      <c r="J6" s="9">
+        <v>0</v>
+      </c>
+      <c r="K6" s="9">
+        <v>0</v>
+      </c>
+      <c r="L6" s="9">
+        <v>0</v>
+      </c>
+      <c r="M6" s="9">
+        <v>0</v>
+      </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
@@ -2541,11 +2582,11 @@
       <c r="E30" s="5"/>
       <c r="F30" s="5">
         <f>SUM(F5:F29)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G30" s="5">
         <f>SUM(G6:G29)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H30" s="5">
         <f t="shared" ref="H30:M30" si="0">SUM(H5:H29)</f>

</xml_diff>

<commit_message>
Updated sprint burndown chart
</commit_message>
<xml_diff>
--- a/Sprint-Backlog-Burndown-Chart.xlsx
+++ b/Sprint-Backlog-Burndown-Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colinconway/Courses/Software_engineering/sandwichTruckProj./"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02212AA2-8FFE-FD49-A601-341ECD151B33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E4257BE-9862-C148-8086-017AAD365B49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="880" windowWidth="25180" windowHeight="14860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="57">
   <si>
     <t>User Story #1</t>
   </si>
@@ -194,6 +194,21 @@
   </si>
   <si>
     <t>Tuesday 3/8</t>
+  </si>
+  <si>
+    <t>Task Priority Queu</t>
+  </si>
+  <si>
+    <t>Task Display Truck</t>
+  </si>
+  <si>
+    <t>Thomas Abatop</t>
+  </si>
+  <si>
+    <t>Task Delivery Route</t>
+  </si>
+  <si>
+    <t>Task UML diagram</t>
   </si>
 </sst>
 </file>
@@ -519,13 +534,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1559,8 +1574,8 @@
   <dimension ref="B1:AC126"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1831,14 +1846,22 @@
     </row>
     <row r="7" spans="2:29" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="9" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
+      <c r="D7" s="9" t="s">
+        <v>35</v>
+      </c>
       <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
+      <c r="F7" s="9">
+        <v>4</v>
+      </c>
+      <c r="G7" s="9">
+        <v>4</v>
+      </c>
+      <c r="H7" s="9">
+        <v>4</v>
+      </c>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
@@ -1863,14 +1886,22 @@
     </row>
     <row r="8" spans="2:29" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="9" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
+      <c r="D8" s="9" t="s">
+        <v>35</v>
+      </c>
       <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
+      <c r="F8" s="9">
+        <v>6</v>
+      </c>
+      <c r="G8" s="9">
+        <v>6</v>
+      </c>
+      <c r="H8" s="9">
+        <v>6</v>
+      </c>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
@@ -1961,13 +1992,19 @@
     </row>
     <row r="11" spans="2:29" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="9" t="s">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
+      <c r="D11" s="9" t="s">
+        <v>54</v>
+      </c>
       <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
+      <c r="F11" s="9">
+        <v>10</v>
+      </c>
+      <c r="G11" s="9">
+        <v>10</v>
+      </c>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
@@ -2123,13 +2160,19 @@
     </row>
     <row r="16" spans="2:29" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="9" t="s">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
+      <c r="D16" s="9" t="s">
+        <v>37</v>
+      </c>
       <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
+      <c r="F16" s="9">
+        <v>8</v>
+      </c>
+      <c r="G16" s="9">
+        <v>8</v>
+      </c>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
@@ -2582,15 +2625,15 @@
       <c r="E30" s="5"/>
       <c r="F30" s="5">
         <f>SUM(F5:F29)</f>
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="G30" s="5">
         <f>SUM(G6:G29)</f>
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="H30" s="5">
         <f t="shared" ref="H30:M30" si="0">SUM(H5:H29)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I30" s="5">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
My Initial Work: Burndown
</commit_message>
<xml_diff>
--- a/Sprint-Backlog-Burndown-Chart.xlsx
+++ b/Sprint-Backlog-Burndown-Chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colinconway/Courses/Software_engineering/sandwichTruckProj./"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abatotmoravian.edu/MyCourses/234/sandwichTruckProj./"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB08FE3-3DAC-E34C-ACBA-F4E1C7675E13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9430C857-B984-8E47-B6F6-227C954CB1E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint Backlog #2" sheetId="8" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="57">
   <si>
     <t>User Story #1</t>
   </si>
@@ -175,24 +175,6 @@
     <t>Task Map</t>
   </si>
   <si>
-    <t>Thursday 3/24</t>
-  </si>
-  <si>
-    <t>Tuesday 3/22</t>
-  </si>
-  <si>
-    <t>Thursday 3/17</t>
-  </si>
-  <si>
-    <t>Tuesday 3/15</t>
-  </si>
-  <si>
-    <t>Thursday 3/10</t>
-  </si>
-  <si>
-    <t>Tuesday 3/8</t>
-  </si>
-  <si>
     <t>Taslk</t>
   </si>
   <si>
@@ -200,6 +182,33 @@
   </si>
   <si>
     <t>Pick Routte Strategy and Have Sandwich Orders</t>
+  </si>
+  <si>
+    <t>Tuesday 3/29</t>
+  </si>
+  <si>
+    <t>Thursday 3/31</t>
+  </si>
+  <si>
+    <t>Tuesday 4/5</t>
+  </si>
+  <si>
+    <t>Thursday 4/7</t>
+  </si>
+  <si>
+    <t>Tuesday 4/11</t>
+  </si>
+  <si>
+    <t>Thursday 4/14</t>
+  </si>
+  <si>
+    <t>Task: Refactor</t>
+  </si>
+  <si>
+    <t>Task: Route Selection GUI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task: Distance Comparator </t>
   </si>
 </sst>
 </file>
@@ -525,7 +534,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1566,7 +1575,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1621,10 +1630,10 @@
     </row>
     <row r="2" spans="2:29" ht="50" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="16" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D2" s="19"/>
       <c r="E2" s="19"/>
@@ -1714,25 +1723,25 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>49</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
@@ -1787,12 +1796,16 @@
     </row>
     <row r="6" spans="2:29" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="9" t="s">
-        <v>2</v>
+        <v>54</v>
       </c>
       <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
+      <c r="D6" s="9" t="s">
+        <v>36</v>
+      </c>
       <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
+      <c r="F6" s="9">
+        <v>4</v>
+      </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
@@ -1819,12 +1832,16 @@
     </row>
     <row r="7" spans="2:29" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="9" t="s">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
+      <c r="D7" s="9" t="s">
+        <v>36</v>
+      </c>
       <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
+      <c r="F7" s="9">
+        <v>4</v>
+      </c>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
@@ -1851,12 +1868,16 @@
     </row>
     <row r="8" spans="2:29" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="9" t="s">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
+      <c r="D8" s="9" t="s">
+        <v>36</v>
+      </c>
       <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
+      <c r="F8" s="9">
+        <v>4</v>
+      </c>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
@@ -1883,7 +1904,7 @@
     </row>
     <row r="9" spans="2:29" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="9" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
@@ -2570,7 +2591,7 @@
       <c r="E30" s="5"/>
       <c r="F30" s="5">
         <f>SUM(F5:F29)</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G30" s="5">
         <f>SUM(G6:G29)</f>

</xml_diff>

<commit_message>
Sprint Burndown Chart ++ Thomas ++ Colin
</commit_message>
<xml_diff>
--- a/Sprint-Backlog-Burndown-Chart.xlsx
+++ b/Sprint-Backlog-Burndown-Chart.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakeclause/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abatotmoravian.edu/MyCourses/234/sandwichTruckProj./"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD68DA5-5232-FD45-864B-1E3DBC944EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74EE47F8-FDE5-5045-84B7-D272222C1A70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="60">
   <si>
     <t>User Story #1</t>
   </si>
@@ -212,6 +212,12 @@
   </si>
   <si>
     <t>Task: Model Sandwich Orders</t>
+  </si>
+  <si>
+    <t>Task: UML Diagram</t>
+  </si>
+  <si>
+    <t>Task: Right Turn Route</t>
   </si>
 </sst>
 </file>
@@ -537,25 +543,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>20</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1577,8 +1583,8 @@
   <dimension ref="B1:AC126"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1809,12 +1815,24 @@
       <c r="F6" s="9">
         <v>4</v>
       </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
+      <c r="G6" s="9">
+        <v>8</v>
+      </c>
+      <c r="H6" s="9">
+        <v>7</v>
+      </c>
+      <c r="I6" s="9">
+        <v>5</v>
+      </c>
+      <c r="J6" s="9">
+        <v>5</v>
+      </c>
+      <c r="K6" s="9">
+        <v>5</v>
+      </c>
+      <c r="L6" s="9">
+        <v>5</v>
+      </c>
       <c r="M6" s="9"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
@@ -1845,12 +1863,24 @@
       <c r="F7" s="9">
         <v>4</v>
       </c>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
+      <c r="G7" s="9">
+        <v>3</v>
+      </c>
+      <c r="H7" s="9">
+        <v>3</v>
+      </c>
+      <c r="I7" s="9">
+        <v>1</v>
+      </c>
+      <c r="J7" s="9">
+        <v>1</v>
+      </c>
+      <c r="K7" s="9">
+        <v>1</v>
+      </c>
+      <c r="L7" s="9">
+        <v>1</v>
+      </c>
       <c r="M7" s="9"/>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
@@ -1881,12 +1911,24 @@
       <c r="F8" s="9">
         <v>4</v>
       </c>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
+      <c r="G8" s="9">
+        <v>4</v>
+      </c>
+      <c r="H8" s="9">
+        <v>4</v>
+      </c>
+      <c r="I8" s="9">
+        <v>4</v>
+      </c>
+      <c r="J8" s="9">
+        <v>4</v>
+      </c>
+      <c r="K8" s="9">
+        <v>4</v>
+      </c>
+      <c r="L8" s="9">
+        <v>4</v>
+      </c>
       <c r="M8" s="9"/>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
@@ -1983,12 +2025,24 @@
       <c r="F11" s="9">
         <v>8</v>
       </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
+      <c r="G11" s="9">
+        <v>7</v>
+      </c>
+      <c r="H11" s="9">
+        <v>5</v>
+      </c>
+      <c r="I11" s="9">
+        <v>3</v>
+      </c>
+      <c r="J11" s="9">
+        <v>3</v>
+      </c>
+      <c r="K11" s="9">
+        <v>3</v>
+      </c>
+      <c r="L11" s="9">
+        <v>3</v>
+      </c>
       <c r="M11" s="9"/>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
@@ -2009,18 +2063,34 @@
     </row>
     <row r="12" spans="2:29" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="9" t="s">
-        <v>2</v>
+        <v>58</v>
       </c>
       <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
+      <c r="D12" s="9" t="s">
+        <v>35</v>
+      </c>
       <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
+      <c r="F12" s="9">
+        <v>6</v>
+      </c>
+      <c r="G12" s="9">
+        <v>6</v>
+      </c>
+      <c r="H12" s="9">
+        <v>6</v>
+      </c>
+      <c r="I12" s="9">
+        <v>6</v>
+      </c>
+      <c r="J12" s="9">
+        <v>6</v>
+      </c>
+      <c r="K12" s="9">
+        <v>6</v>
+      </c>
+      <c r="L12" s="9">
+        <v>6</v>
+      </c>
       <c r="M12" s="9"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
@@ -2041,18 +2111,34 @@
     </row>
     <row r="13" spans="2:29" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="9" t="s">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
+      <c r="D13" s="9" t="s">
+        <v>35</v>
+      </c>
       <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
+      <c r="F13" s="9">
+        <v>12</v>
+      </c>
+      <c r="G13" s="9">
+        <v>12</v>
+      </c>
+      <c r="H13" s="9">
+        <v>12</v>
+      </c>
+      <c r="I13" s="9">
+        <v>10</v>
+      </c>
+      <c r="J13" s="9">
+        <v>10</v>
+      </c>
+      <c r="K13" s="9">
+        <v>10</v>
+      </c>
+      <c r="L13" s="9">
+        <v>10</v>
+      </c>
       <c r="M13" s="9"/>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
@@ -2600,31 +2686,31 @@
       <c r="E30" s="5"/>
       <c r="F30" s="5">
         <f>SUM(F5:F29)</f>
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="G30" s="5">
         <f>SUM(G6:G29)</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="H30" s="5">
         <f t="shared" ref="H30:M30" si="0">SUM(H5:H29)</f>
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="I30" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="J30" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="K30" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="L30" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="M30" s="5">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Burndown Colin and Thomas
</commit_message>
<xml_diff>
--- a/Sprint-Backlog-Burndown-Chart.xlsx
+++ b/Sprint-Backlog-Burndown-Chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abatotmoravian.edu/MyCourses/234/sandwichTruckProj./"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/conwaycmoravian.edu/Courses/234/sandwichTruckProj./"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74EE47F8-FDE5-5045-84B7-D272222C1A70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2CAC17B-141E-AD46-A22C-5FD41E23BA70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint Backlog #2" sheetId="8" r:id="rId1"/>
@@ -555,16 +555,16 @@
                   <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>29</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>29</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>29</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1583,7 +1583,7 @@
   <dimension ref="B1:AC126"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
@@ -1833,7 +1833,9 @@
       <c r="L6" s="9">
         <v>5</v>
       </c>
-      <c r="M6" s="9"/>
+      <c r="M6" s="9">
+        <v>5</v>
+      </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
@@ -1881,7 +1883,9 @@
       <c r="L7" s="9">
         <v>1</v>
       </c>
-      <c r="M7" s="9"/>
+      <c r="M7" s="9">
+        <v>1</v>
+      </c>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
@@ -1929,7 +1933,9 @@
       <c r="L8" s="9">
         <v>4</v>
       </c>
-      <c r="M8" s="9"/>
+      <c r="M8" s="9">
+        <v>4</v>
+      </c>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
@@ -2035,15 +2041,17 @@
         <v>3</v>
       </c>
       <c r="J11" s="9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K11" s="9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L11" s="9">
-        <v>3</v>
-      </c>
-      <c r="M11" s="9"/>
+        <v>0</v>
+      </c>
+      <c r="M11" s="9">
+        <v>0</v>
+      </c>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
@@ -2091,7 +2099,9 @@
       <c r="L12" s="9">
         <v>6</v>
       </c>
-      <c r="M12" s="9"/>
+      <c r="M12" s="9">
+        <v>6</v>
+      </c>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
@@ -2134,12 +2144,14 @@
         <v>10</v>
       </c>
       <c r="K13" s="9">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="L13" s="9">
-        <v>10</v>
-      </c>
-      <c r="M13" s="9"/>
+        <v>4</v>
+      </c>
+      <c r="M13" s="9">
+        <v>4</v>
+      </c>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
@@ -2702,19 +2714,19 @@
       </c>
       <c r="J30" s="5">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K30" s="5">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="L30" s="5">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="M30" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="N30" s="4"/>
       <c r="O30" s="4"/>

</xml_diff>